<commit_message>
Fixed the sheet with accurate data
</commit_message>
<xml_diff>
--- a/nodes.xlsx
+++ b/nodes.xlsx
@@ -1,70 +1,158 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4AA7320-9C62-436F-8D5E-C8A6D79EBDEF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JackD\Desktop\QHacks\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{765322B9-B430-4890-905D-62CFCC4A5081}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17630" windowHeight="4170" xr2:uid="{146BF8FD-DCB6-444C-BF10-DFFF515EBC55}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
-  <si>
-    <t>43.659815, -79.390429</t>
-  </si>
-  <si>
-    <t>43.660839, -79.385869</t>
-  </si>
-  <si>
-    <t>43.661441, -79.383075</t>
-  </si>
-  <si>
-    <t>43.659120, -79.382163</t>
-  </si>
-  <si>
-    <t>43.658499, -79.384834</t>
-  </si>
-  <si>
-    <t>43.657591, -79.389331</t>
-  </si>
-  <si>
-    <t>43.652879, -79.397979</t>
-  </si>
-  <si>
-    <t>43.651295, -79.405618</t>
-  </si>
-  <si>
-    <t>43.647258, -79.404031</t>
-  </si>
-  <si>
-    <t>43.648748, -79.396349</t>
-  </si>
-  <si>
-    <t>43.650812, -79.386606</t>
-  </si>
-  <si>
-    <t>43.650469, -79.378517</t>
-  </si>
-  <si>
-    <t>43.649910, -79.380792</t>
-  </si>
-  <si>
-    <t>43.648885, -79.385684</t>
-  </si>
-  <si>
-    <t>43.646308, -79.391091</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+  <si>
+    <t>jarvis</t>
+  </si>
+  <si>
+    <t>sherborne</t>
+  </si>
+  <si>
+    <t>parliament</t>
+  </si>
+  <si>
+    <t>church</t>
+  </si>
+  <si>
+    <t>yonge</t>
+  </si>
+  <si>
+    <t>wellesley</t>
+  </si>
+  <si>
+    <t>carlton</t>
+  </si>
+  <si>
+    <t>gerrard</t>
+  </si>
+  <si>
+    <t>dundas</t>
+  </si>
+  <si>
+    <t>queen</t>
+  </si>
+  <si>
+    <t>bay</t>
+  </si>
+  <si>
+    <t>43.664356, -79.387163</t>
+  </si>
+  <si>
+    <t>43.660837, -79.385846</t>
+  </si>
+  <si>
+    <t>43.658455, -79.384852</t>
+  </si>
+  <si>
+    <t>43.655775, -79.383666</t>
+  </si>
+  <si>
+    <t>43.651870, -79.381810</t>
+  </si>
+  <si>
+    <t>43.652448, -79.379307</t>
+  </si>
+  <si>
+    <t>43.656292, -79.380896</t>
+  </si>
+  <si>
+    <t>43.659094, -79.382114</t>
+  </si>
+  <si>
+    <t>43.661403, -79.383101</t>
+  </si>
+  <si>
+    <t>43.664932, -79.384514</t>
+  </si>
+  <si>
+    <t>43.665730, -79.380942</t>
+  </si>
+  <si>
+    <t>43.661898, -79.379297</t>
+  </si>
+  <si>
+    <t>43.659910, -79.378477</t>
+  </si>
+  <si>
+    <t>43.656518, -79.377131</t>
+  </si>
+  <si>
+    <t>43.653161, -79.375726</t>
+  </si>
+  <si>
+    <t>43.653713, -79.373216</t>
+  </si>
+  <si>
+    <t>43.657050, -79.374553</t>
+  </si>
+  <si>
+    <t>43.660467, -79.375801</t>
+  </si>
+  <si>
+    <t>43.662422, -79.376687</t>
+  </si>
+  <si>
+    <t>43.666264, -79.378328</t>
+  </si>
+  <si>
+    <t>43.667071, -79.374680</t>
+  </si>
+  <si>
+    <t>43.663183, -79.373071</t>
+  </si>
+  <si>
+    <t>43.661243, -79.372213</t>
+  </si>
+  <si>
+    <t>43.658301, -79.370947</t>
+  </si>
+  <si>
+    <t>43.654510, -79.369440</t>
+  </si>
+  <si>
+    <t>43.655605, -79.364435</t>
+  </si>
+  <si>
+    <t>43.659381, -79.365975</t>
+  </si>
+  <si>
+    <t>43.662322, -79.367185</t>
+  </si>
+  <si>
+    <t>43.664295, -79.367982</t>
+  </si>
+  <si>
+    <t>43.668180, -79.369546</t>
   </si>
 </sst>
 </file>
@@ -100,11 +188,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -139,7 +226,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -151,7 +238,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -198,6 +285,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -233,6 +337,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -384,75 +505,152 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECFBEF55-FF1D-4377-B18D-D2B7B3422969}">
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="20.109375" customWidth="1"/>
-    <col min="3" max="3" width="19.5546875" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" customWidth="1"/>
+    <col min="1" max="6" width="19.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added cars to the nodes
</commit_message>
<xml_diff>
--- a/nodes.xlsx
+++ b/nodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JackD\Desktop\QHacks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBCF6AA-10F0-406D-9E14-1C3404B9F43B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B25CB68-84BC-4F0E-8A82-CBD44E04C125}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17630" windowHeight="4170" activeTab="1" xr2:uid="{146BF8FD-DCB6-444C-BF10-DFFF515EBC55}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
   <si>
     <t>jarvis</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t>43.668180, -79.369546</t>
-  </si>
-  <si>
-    <t>tset</t>
   </si>
 </sst>
 </file>
@@ -513,7 +510,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScale="70" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B5" sqref="B5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -665,17 +662,105 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{969B8455-8D93-4AC5-BA64-FDEA5E56C09E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>41</v>
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IT IS WORKING MOTHAPOOPERS
</commit_message>
<xml_diff>
--- a/nodes.xlsx
+++ b/nodes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JackD\Desktop\QHacks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\QHacks2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B25CB68-84BC-4F0E-8A82-CBD44E04C125}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAECEAD-EBA1-4F09-BF79-404C4C005D79}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17630" windowHeight="4170" activeTab="1" xr2:uid="{146BF8FD-DCB6-444C-BF10-DFFF515EBC55}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17628" windowHeight="4176" xr2:uid="{146BF8FD-DCB6-444C-BF10-DFFF515EBC55}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,40 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
-  <si>
-    <t>jarvis</t>
-  </si>
-  <si>
-    <t>sherborne</t>
-  </si>
-  <si>
-    <t>parliament</t>
-  </si>
-  <si>
-    <t>church</t>
-  </si>
-  <si>
-    <t>yonge</t>
-  </si>
-  <si>
-    <t>wellesley</t>
-  </si>
-  <si>
-    <t>carlton</t>
-  </si>
-  <si>
-    <t>gerrard</t>
-  </si>
-  <si>
-    <t>dundas</t>
-  </si>
-  <si>
-    <t>queen</t>
-  </si>
-  <si>
-    <t>bay</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>43.664356, -79.387163</t>
   </si>
@@ -102,9 +69,6 @@
     <t>43.661898, -79.379297</t>
   </si>
   <si>
-    <t>43.659910, -79.378477</t>
-  </si>
-  <si>
     <t>43.656518, -79.377131</t>
   </si>
   <si>
@@ -154,6 +118,12 @@
   </si>
   <si>
     <t>43.668180, -79.369546</t>
+  </si>
+  <si>
+    <t>0,0</t>
+  </si>
+  <si>
+    <t>43.659094, -79.3822</t>
   </si>
 </sst>
 </file>
@@ -507,151 +477,121 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECFBEF55-FF1D-4377-B18D-D2B7B3422969}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView zoomScale="70" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:E5"/>
+    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="19.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="6" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F11" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -664,103 +604,101 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{969B8455-8D93-4AC5-BA64-FDEA5E56C09E}">
   <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>